<commit_message>
password to download file works good
</commit_message>
<xml_diff>
--- a/Desktop/IPtv_projects/Projects Eldad/Bot/uploaded_files.xlsx
+++ b/Desktop/IPtv_projects/Projects Eldad/Bot/uploaded_files.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -935,6 +935,81 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>IsraTv2203.m3u</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>GroupAnonymousBot</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1087968824</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Playlists</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2025-03-22 22:58:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>EGlayList230325.m3u</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>GroupAnonymousBot</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1087968824</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Playlists</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2025-03-23 18:42:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>EGlayList230325.m3u</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>GroupAnonymousBot</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1087968824</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Playlists</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2025-03-23 18:45:17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>